<commit_message>
files for (c) Stability
</commit_message>
<xml_diff>
--- a/Graphs/Time_step_length_N_bodies_RK4.xlsx
+++ b/Graphs/Time_step_length_N_bodies_RK4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Birgitte\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Birgitte\Documents\GitHub\Project5\Graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10788" windowHeight="8640" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10788" windowHeight="8640" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Ark6" sheetId="6" r:id="rId6"/>
     <sheet name="Ark7" sheetId="7" r:id="rId7"/>
     <sheet name="Ark8" sheetId="8" r:id="rId8"/>
+    <sheet name="Ark9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="11">
   <si>
     <t>dt = 10^4 yr</t>
   </si>
@@ -8940,7 +8941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -9768,4 +9769,833 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>19.681000000000001</v>
+      </c>
+      <c r="B3">
+        <v>4.7068099999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7.2486899999999999</v>
+      </c>
+      <c r="B4">
+        <v>3.7665099999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>12.0977</v>
+      </c>
+      <c r="B5">
+        <v>3492.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>14.4453</v>
+      </c>
+      <c r="B6">
+        <v>6.2738100000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>18.603899999999999</v>
+      </c>
+      <c r="B7">
+        <v>5.0152000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>16.677099999999999</v>
+      </c>
+      <c r="B8">
+        <v>6.8936599999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>18.3157</v>
+      </c>
+      <c r="B9">
+        <v>7.00631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>12.977</v>
+      </c>
+      <c r="B10">
+        <v>4.1956499999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>14.9846</v>
+      </c>
+      <c r="B11">
+        <v>41.105400000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>17.848500000000001</v>
+      </c>
+      <c r="B12">
+        <v>5.2284100000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15.5824</v>
+      </c>
+      <c r="B13">
+        <v>12.452199999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>15.7865</v>
+      </c>
+      <c r="B14">
+        <v>5.6434699999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>13.893700000000001</v>
+      </c>
+      <c r="B15">
+        <v>22.733899999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>19.9543</v>
+      </c>
+      <c r="B16">
+        <v>6.6444400000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>18.941500000000001</v>
+      </c>
+      <c r="B17">
+        <v>6.9756299999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>19.6629</v>
+      </c>
+      <c r="B18">
+        <v>33.0413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>11.982100000000001</v>
+      </c>
+      <c r="B19">
+        <v>4.9547600000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19.337199999999999</v>
+      </c>
+      <c r="B20">
+        <v>10.2332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4.5030700000000001</v>
+      </c>
+      <c r="B21">
+        <v>1.4656100000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>14.4718</v>
+      </c>
+      <c r="B22">
+        <v>56.599800000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>10.851000000000001</v>
+      </c>
+      <c r="B23">
+        <v>255.70099999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>13.364100000000001</v>
+      </c>
+      <c r="B24">
+        <v>23.469100000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>16.158999999999999</v>
+      </c>
+      <c r="B25">
+        <v>19.7639</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>19.143699999999999</v>
+      </c>
+      <c r="B26">
+        <v>12.083399999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>18.476500000000001</v>
+      </c>
+      <c r="B27">
+        <v>4.6040000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>17.917200000000001</v>
+      </c>
+      <c r="B28">
+        <v>49.410699999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>12.2585</v>
+      </c>
+      <c r="B29">
+        <v>39.158299999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>17.616099999999999</v>
+      </c>
+      <c r="B30">
+        <v>6.8544099999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>16.656300000000002</v>
+      </c>
+      <c r="B31">
+        <v>11.2644</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>19.308599999999998</v>
+      </c>
+      <c r="B32">
+        <v>7.0667799999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>17.760899999999999</v>
+      </c>
+      <c r="B33">
+        <v>6.52996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>18.191600000000001</v>
+      </c>
+      <c r="B34">
+        <v>28.668600000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>14.968999999999999</v>
+      </c>
+      <c r="B35">
+        <v>62.945099999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>13.582800000000001</v>
+      </c>
+      <c r="B36">
+        <v>4.2919900000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>17.247</v>
+      </c>
+      <c r="B37">
+        <v>5.3877100000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>12.285500000000001</v>
+      </c>
+      <c r="B38">
+        <v>40.470599999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>19.0854</v>
+      </c>
+      <c r="B39">
+        <v>2.8316699999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>9.3107699999999998</v>
+      </c>
+      <c r="B40">
+        <v>107.08499999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>19.0733</v>
+      </c>
+      <c r="B41">
+        <v>5.75793</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>15.1214</v>
+      </c>
+      <c r="B42">
+        <v>124.812</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>7.46957</v>
+      </c>
+      <c r="B43">
+        <v>5.6046100000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>12.3087</v>
+      </c>
+      <c r="B44">
+        <v>3.5590999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>9.8798499999999994</v>
+      </c>
+      <c r="B45">
+        <v>6.3836599999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>14.5817</v>
+      </c>
+      <c r="B46">
+        <v>6.3193799999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>17.730399999999999</v>
+      </c>
+      <c r="B47">
+        <v>7.2483500000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>12.443099999999999</v>
+      </c>
+      <c r="B48">
+        <v>122.523</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>15.176</v>
+      </c>
+      <c r="B49">
+        <v>4.9315100000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>16.822099999999999</v>
+      </c>
+      <c r="B50">
+        <v>106.18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>12.8066</v>
+      </c>
+      <c r="B51">
+        <v>5.1778199999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>14.272</v>
+      </c>
+      <c r="B52">
+        <v>7.3676899999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>13.081099999999999</v>
+      </c>
+      <c r="B53">
+        <v>2642.07</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>6.2914599999999998</v>
+      </c>
+      <c r="B54">
+        <v>1.0716300000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>17.182200000000002</v>
+      </c>
+      <c r="B55">
+        <v>47.158999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>15.3965</v>
+      </c>
+      <c r="B56">
+        <v>4.4881200000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>10.865500000000001</v>
+      </c>
+      <c r="B57">
+        <v>28.571000000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>6.6582499999999998</v>
+      </c>
+      <c r="B58">
+        <v>38.154400000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>14.055</v>
+      </c>
+      <c r="B59">
+        <v>6.4270199999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>15.892899999999999</v>
+      </c>
+      <c r="B60">
+        <v>5.2398600000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>19.744700000000002</v>
+      </c>
+      <c r="B61">
+        <v>7.9282700000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>10.986800000000001</v>
+      </c>
+      <c r="B62">
+        <v>3.70994</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>18.695900000000002</v>
+      </c>
+      <c r="B63">
+        <v>5.5580299999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>8.1631199999999993</v>
+      </c>
+      <c r="B64">
+        <v>3.8704100000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>17.677499999999998</v>
+      </c>
+      <c r="B65">
+        <v>49.976599999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>16.760100000000001</v>
+      </c>
+      <c r="B66">
+        <v>297.13099999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>16.262799999999999</v>
+      </c>
+      <c r="B67">
+        <v>4.4987000000000004</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>16.4634</v>
+      </c>
+      <c r="B68">
+        <v>33.192500000000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>19.045500000000001</v>
+      </c>
+      <c r="B69">
+        <v>7.5705</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>10.575100000000001</v>
+      </c>
+      <c r="B70">
+        <v>83.69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>17.932600000000001</v>
+      </c>
+      <c r="B71">
+        <v>209.999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>16.802299999999999</v>
+      </c>
+      <c r="B72">
+        <v>4.6197999999999997</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>12.851100000000001</v>
+      </c>
+      <c r="B73">
+        <v>2.9603600000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>17.397300000000001</v>
+      </c>
+      <c r="B74">
+        <v>6.0581100000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>13.985799999999999</v>
+      </c>
+      <c r="B75">
+        <v>3.7327300000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>14.4496</v>
+      </c>
+      <c r="B76">
+        <v>3.9341900000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>13.061</v>
+      </c>
+      <c r="B77">
+        <v>6.9902800000000003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>16.309699999999999</v>
+      </c>
+      <c r="B78">
+        <v>5.33439</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>8.00624</v>
+      </c>
+      <c r="B79">
+        <v>2.6654200000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>14.492699999999999</v>
+      </c>
+      <c r="B80">
+        <v>166.06800000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>16.044799999999999</v>
+      </c>
+      <c r="B81">
+        <v>6.1206699999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>14.7384</v>
+      </c>
+      <c r="B82">
+        <v>5.0501699999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>3.9839799999999999</v>
+      </c>
+      <c r="B83">
+        <v>4.26891</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>11.5158</v>
+      </c>
+      <c r="B84">
+        <v>220.285</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>19.808599999999998</v>
+      </c>
+      <c r="B85">
+        <v>6.05532</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>16.898900000000001</v>
+      </c>
+      <c r="B86">
+        <v>5.0494599999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>18.830200000000001</v>
+      </c>
+      <c r="B87">
+        <v>5.26485</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>19.125299999999999</v>
+      </c>
+      <c r="B88">
+        <v>5.8116899999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>14.7654</v>
+      </c>
+      <c r="B89">
+        <v>5.53878</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>15.951599999999999</v>
+      </c>
+      <c r="B90">
+        <v>143.041</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>9.6877099999999992</v>
+      </c>
+      <c r="B91">
+        <v>4.9323699999999997</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>17.671500000000002</v>
+      </c>
+      <c r="B92">
+        <v>209.267</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>11.144299999999999</v>
+      </c>
+      <c r="B93">
+        <v>5.14154</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>14.476800000000001</v>
+      </c>
+      <c r="B94">
+        <v>24.183499999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>15.232699999999999</v>
+      </c>
+      <c r="B95">
+        <v>164.14400000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>15.8706</v>
+      </c>
+      <c r="B96">
+        <v>50.3489</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>12.898300000000001</v>
+      </c>
+      <c r="B97">
+        <v>3.76993</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>17.137699999999999</v>
+      </c>
+      <c r="B98">
+        <v>259.84300000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>13.122299999999999</v>
+      </c>
+      <c r="B99">
+        <v>3.32524</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>17.953099999999999</v>
+      </c>
+      <c r="B100">
+        <v>5.9745600000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>17.761700000000001</v>
+      </c>
+      <c r="B101">
+        <v>3.4159299999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>15.257899999999999</v>
+      </c>
+      <c r="B102">
+        <v>4.0402199999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>